<commit_message>
adds auc and calibration
</commit_message>
<xml_diff>
--- a/predictions/predictions.xlsx
+++ b/predictions/predictions.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demetri/gitrepos/Euro2020/predictions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{23FE1F09-C9A0-D849-BC07-DDB1B17E5A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2DE5096-2414-3E43-9BF7-F84CC65B5C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340"/>
+    <workbookView xWindow="76780" yWindow="3560" windowWidth="25600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="predictions" sheetId="1" r:id="rId1"/>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -792,7 +792,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -829,6 +828,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1042,33 +1042,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:P37" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:P37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:P37" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" name="Group" dataDxfId="17"/>
-    <tableColumn id="2" name="teamA" dataDxfId="16"/>
-    <tableColumn id="3" name="teamB" dataDxfId="15"/>
-    <tableColumn id="4" name="A Wins" dataDxfId="14"/>
-    <tableColumn id="5" name="B Wins" dataDxfId="13"/>
-    <tableColumn id="6" name="Draw" dataDxfId="12"/>
-    <tableColumn id="7" name="Awon" dataDxfId="9"/>
-    <tableColumn id="8" name="Bwon" dataDxfId="8"/>
-    <tableColumn id="9" name="DrawHappened" dataDxfId="7"/>
-    <tableColumn id="10" name="LossA" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Group" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="teamA" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="teamB" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="A Wins" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="B Wins" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Draw" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Awon" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Bwon" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="DrawHappened" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="LossA" dataDxfId="6">
       <calculatedColumnFormula>-LOG(Table1[[#This Row],[A Wins]],EXP(1))*Table1[[#This Row],[Awon]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="LossB" dataDxfId="6">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="LossB" dataDxfId="5">
       <calculatedColumnFormula>-LOG(Table1[[#This Row],[B Wins]],EXP(1))*Table1[[#This Row],[Bwon]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="LossDraw" dataDxfId="5">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="LossDraw" dataDxfId="4">
       <calculatedColumnFormula>-LOG(Table1[[#This Row],[Draw]],EXP(1))*Table1[[#This Row],[DrawHappened]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Loss" dataDxfId="3">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Loss" dataDxfId="3">
       <calculatedColumnFormula>SUM(Table1[[#This Row],[LossA]:[LossDraw]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="ScoreA" dataDxfId="2"/>
-    <tableColumn id="16" name="ScoreB" dataDxfId="1"/>
-    <tableColumn id="17" name="Random Guessing" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="ScoreA" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="ScoreB" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Random Guessing" dataDxfId="0">
       <calculatedColumnFormula>-LOG(0.33, EXP(1))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1372,11 +1372,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P37"/>
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,8 +1524,12 @@
         <f>SUM(Table1[[#This Row],[LossA]:[LossDraw]])</f>
         <v>0</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
       <c r="P3" s="1">
         <f t="shared" si="0"/>
         <v>1.1086626245216111</v>
@@ -1640,9 +1644,15 @@
       <c r="F6" s="1">
         <v>0.20799999999999999</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
       <c r="J6" s="1">
         <f>-LOG(Table1[[#This Row],[A Wins]],EXP(1))*Table1[[#This Row],[Awon]]</f>
         <v>0</v>
@@ -1653,14 +1663,18 @@
       </c>
       <c r="L6" s="1">
         <f>-LOG(Table1[[#This Row],[Draw]],EXP(1))*Table1[[#This Row],[DrawHappened]]</f>
-        <v>0</v>
+        <v>1.5702171992808192</v>
       </c>
       <c r="M6" s="1">
         <f>SUM(Table1[[#This Row],[LossA]:[LossDraw]])</f>
-        <v>0</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+        <v>1.5702171992808192</v>
+      </c>
+      <c r="N6" s="1">
+        <v>1</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
       <c r="P6" s="1">
         <f t="shared" si="0"/>
         <v>1.1086626245216111</v>
@@ -1820,12 +1834,18 @@
       <c r="F10" s="1">
         <v>0.17674999999999999</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
       <c r="J10" s="1">
         <f>-LOG(Table1[[#This Row],[A Wins]],EXP(1))*Table1[[#This Row],[Awon]]</f>
-        <v>0</v>
+        <v>0.42656107140289873</v>
       </c>
       <c r="K10" s="1">
         <f>-LOG(Table1[[#This Row],[B Wins]],EXP(1))*Table1[[#This Row],[Bwon]]</f>
@@ -1837,10 +1857,14 @@
       </c>
       <c r="M10" s="1">
         <f>SUM(Table1[[#This Row],[LossA]:[LossDraw]])</f>
-        <v>0</v>
-      </c>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+        <v>0.42656107140289873</v>
+      </c>
+      <c r="N10" s="1">
+        <v>3</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
       <c r="P10" s="1">
         <f t="shared" si="0"/>
         <v>1.1086626245216111</v>
@@ -1865,16 +1889,22 @@
       <c r="F11" s="1">
         <v>0.17974999999999999</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
       <c r="J11" s="1">
         <f>-LOG(Table1[[#This Row],[A Wins]],EXP(1))*Table1[[#This Row],[Awon]]</f>
         <v>0</v>
       </c>
       <c r="K11" s="1">
         <f>-LOG(Table1[[#This Row],[B Wins]],EXP(1))*Table1[[#This Row],[Bwon]]</f>
-        <v>0</v>
+        <v>1.6309169441112246</v>
       </c>
       <c r="L11" s="1">
         <f>-LOG(Table1[[#This Row],[Draw]],EXP(1))*Table1[[#This Row],[DrawHappened]]</f>
@@ -1882,10 +1912,14 @@
       </c>
       <c r="M11" s="1">
         <f>SUM(Table1[[#This Row],[LossA]:[LossDraw]])</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+        <v>1.6309169441112246</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1</v>
+      </c>
       <c r="P11" s="1">
         <f t="shared" si="0"/>
         <v>1.1086626245216111</v>

</xml_diff>

<commit_message>
adds some ROC stuff
</commit_message>
<xml_diff>
--- a/predictions/predictions.xlsx
+++ b/predictions/predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/demetri/gitrepos/Euro2020/predictions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{596B6C42-BA6A-1640-A2D6-EE163804C152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4145DD6F-1750-1943-90D2-4D472E3F90CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20120" yWindow="9900" windowWidth="27640" windowHeight="16940"/>
   </bookViews>
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1105,27 +1105,27 @@
         <v>0.17374999999999999</v>
       </c>
       <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>3</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
         <f>-LOG(Table2[[#This Row],[A Wins]], EXP(1))*Table2[[#This Row],[Awon]]</f>
-        <v>1.7189737995024073</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <f>-LOG(Table2[[#This Row],[B Wins]], EXP(1))*Table2[[#This Row],[Bwon]]</f>
-        <v>0</v>
+        <v>0.43540898448123644</v>
       </c>
       <c r="N2">
         <f>-LOG(Table2[[#This Row],[Draw]], EXP(1))*Table2[[#This Row],[NeitherWon]]</f>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="O2">
         <f>SUM(Table2[[#This Row],[LossA]:[LossDraw]])</f>
-        <v>1.7189737995024073</v>
+        <v>0.43540898448123644</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>